<commit_message>
Separe as letras das músicas e retire as virgulas
</commit_message>
<xml_diff>
--- a/excel/A1 LP.xlsx
+++ b/excel/A1 LP.xlsx
@@ -15,14 +15,14 @@
     <sheet name="EdSheeran" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">EdSheeran!$A$1:$F$135</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">EdSheeran!$A$1:$F$134</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="284">
   <si>
     <t>Artista</t>
   </si>
@@ -294,12 +294,6 @@
     <t>i should ink my skin with your name and take my passport out again and just replace it see i could do without a tan on my left hand where my fourth finger meets my knuckle and i should run you a hot bath fill it up with bubbles 'cause maybe you're loveable maybe you're my snowflake and your eyes turn from green to gray and in the winter i'll hold you in a cold place and you should never cut your hair 'cause i love the way you flick it off your shoulder  hook and you will never know just how beautiful you are to me but maybe i'm just in love when you wake me up   and would you ever feel guilty if you did the same to me could you make me a cup of tea to open my eyes in the right way and i know you love shrek 'cause we've watched it  times and maybe you're hoping for a fairytale too and if your dvd breaks today you should've got a vcr because i've never owned a bluray true say i know i've always been shit at computer games and your brother always beats me and if i lost i go across and chuck all the controllers at the tv and then you laugh at me and be asking me if i'm gonna be home next week and then you lie with me 'til i fall asleep and flutter eye lash on my cheek between the sheets  hook and you will never know just how beautiful you are to me but maybe i'm just in love when you wake me up   and i think you hate the smell of smoke you always try and get me to stop but you drink as much as me and i get drunk a lot so ill take you to the beach and walk along the sand and i'll make you a heart pendant with a pebble held in my hand and i'll carve it like this necklace so the heart falls where your chest is now a piece of me is a piece of the beach and it falls just where it needs to be and rests peacefully so you just need to breathe to feel my heart against yours now against yours now cos maybe i'm just in love when you wake me up or maybe i'm just in love when you wake me up maybe i fell in love when you woke me up</t>
   </si>
   <si>
-    <t>All of the Stars</t>
-  </si>
-  <si>
-    <t>it's just another night and i'm staring at the moon i saw a shooting star and thought of you i sang a lullaby by the waterside and knew if you were here i'd sing to you you're on the other side as the skyline splits in two i'm miles away from seeing you but i can see the stars from america i wondered do you see them too   so open your eyes and see the way our horizons meet and all of the lights will lead into the night with me and i know these scars will bleed but both of our hearts believe all of these stars will guide us home   i can hear your heart on the radio beat they're playing chasing cars and i thought of us back to the time you were lying next to me i looked across and fell in love so i took your hand back through lamp lit streets i knew everything led back to you so can you see the stars over amsterdam you're the song my heart is beating to   so open your eyes and see the way our horizons meet and all of the lights will lead into the night with me and i know these scars will bleed but both of our hearts believe all of these stars will guide us home   and oh i know and oh i know and oh i can see the stars from america</t>
-  </si>
-  <si>
     <t>The Man</t>
   </si>
   <si>
@@ -768,9 +762,6 @@
     <t>Peru</t>
   </si>
   <si>
-    <t>The Fault In Our Stars</t>
-  </si>
-  <si>
     <t>I Don't Care</t>
   </si>
   <si>
@@ -822,661 +813,952 @@
     <t>you know i got to get away to find some peace and sanity ive been playing hideandseek too long shaking making everybody waking setting the hifi bleed keeping me back while youre spinning my track thatll knock you off your feet monkey see what monkey do but im a monkey telling you i just think that we should take a break tickitytock the clock with the hiphop and alonestar backing me up we wont stop i gotta be searching for my peace of mind now let the track rewind  hook ed sheeran and play let the music play it came so let the music say what it feels shame shame it took too long to see that you were wrong now turn the song back on   this is alonestar coming at you with a new style kicking dust ready to bust it's urban angel artistic flipping the script who'd you really want to get it with ed and alonestar we're like live wires sparking ready to blow we've already sown our seeds we're just waiting to grow blow we're gonna lift you like a shock to your body metaphorical speech when we come and see you ducking for cover sheeran lock coming ready to rock with urban angel and alonestar and ed keep it locked let the beat pump drop the bass but don't stop we're kicking the sound let the bass bins pound we're gonna roll can you feel me now with my body get down to the sound it's ed sheeran in the place and alonestar rising up we gotta rise up i said rise up  hook</t>
   </si>
   <si>
-    <t>I have grown up, I am a father now
-Everything has changed, but I am still the same somehow
-You know I've never been afraid of death
-But now I wanna see the things that haven't happened yet
-I still love getting out of my mind, I should cut it down
-I still know people I don't like and I should cut them out
-I feel embarrassed 'bout the things that I did in my youth
-'Cause now I have a child, I know one day that you will do it
-Freight cargo, dot stops and aeroplanes
-Late-night calls, signal is in and out again
-Feelin' low, serotonin known better days
-Go, go, go! But every moment you're here with me
-Timе stops to still
-When you are in my arms, it always will
-And life, lifе is changin' tides
-I lost the confidence in who I was
-Too busy tryna chase the high and get the numbers up
-I have the same dream every night
-A bullet through my brain the moment that I close my eyes
-I still have to lean on a shoulder when I've broken down
-And I have people that depend on me to sort them out
-I sometimes fantasize I disappear without a trace
-I've no regrets, but wish I did things in a different way
-Low fly zone, lawsuits, and film stars
-Headline wrote the princess and the face scar
-Broken bones, break-ins, and Babylon
-Go, go, go! But every moment you're here with me
-Time stops to still
-When you are in my arms, it always will
-And life, life is changin' tides
-Time stops to still
-When you are in my arms, it always will
-And life, life is changin' tides</t>
-  </si>
-  <si>
-    <t>I took an arrow to the heart
-I never kissed a mouth that tastes like yours
-Strawberries and somethin' more
-Ooh yeah, I want it all
-Lipstick on my guitar (ooh)
-Fill up the engine, we can drive real far
-Go dancin' underneath the stars
-Ooh yeah, I want it all
-Mm, you got me feelin' like
-I wanna be that guy, I wanna kiss your eyes
-I wanna drink that smile, I wanna feel like I'm
-Like my soul's on fire, I wanna stay up all day and all night
-Yeah, you got me singin' like
-Ooh, I love it when you do it like that
-And when you're close up, give me the shivers
-Oh baby, you wanna dance 'til the sunlight cracks
-And when they say the party's over, then we'll bring it right back
-And we'll say, ooh, I love it when you do it like that
-And when you're close up, give me the shivers
-Oh baby, you wanna dance 'til the sunlight cracks
-And when they say the party's over, then we'll bring it right back
-Into the car
-On the backseat in the moonlit dark
-Wrap me up between your legs and arms
-Ooh, I can't get enough
-You know you could tear me apart (ooh)
-Put me back together and take my heart
-I never thought that I could love this hard
-Ooh, I can't get enough
-Mm, you got me feeling like
-I wanna be that guy, I wanna kiss your eyes
-I wanna drink that smile, I wanna feel like I'm
-Like my soul's on fire, I wanna stay up all day and all night
-Yeah, you got me singin' like
-Ooh, I love it when you do it like that
-And when you're close up, give me the shivers
-Oh baby, you wanna dance 'til the sunlight cracks
-And when they say the party's over, then we'll bring it right back
-And we'll say, ooh, I love it when you do it like that
-And when you're close up, give me the shivers
-Oh baby, you wanna dance 'til the sunlight cracks
-And when they say the party's over, then we'll bring it right back
-Baby, you burn so hot
-You make me shiver with the fire you got
-This thing we started, I don't want it to stop
-You know you make me shiver-er-er
-Baby, you burn so hot
-You make me shiver with the fire you got
-This thing we started, I don't want it to stop
-You know you make me shiver
-Yeah, you got me singin' like
-Ooh, I love it when you do it like that
-And when you're close up, give me the shivers
-Oh baby, you wanna dance 'til the sunlight cracks
-And when they say the party's over, then we'll bring it right back (oh no)
-And we'll say, ooh, I love it when you do it like that
-And when you're close up, give me the shivers
-Oh baby, you wanna dance 'til the sunlight cracks
-And when they say the party's over, then we'll bring it right back, hey</t>
-  </si>
-  <si>
-    <t>I thought it'd feel different, playin' Wembley
-Eighty thousand singin' with me
-It's what I've been chasin' 'cause this is the dream
-When it was all over, I cleared out the room
-Grabbed a couple beers, just me and you
-Then we started talking the way that we do
-Ain't it funny how the simplest things in life can make a man?
-Little moments that pass us by
-Oh, but I remember
-The first kiss, the first night, the first song that made you cry
-The first drink, red wine, on a step in Brooklyn, I
-Still feel the first fight, and we both made it out alive
-And I can't wait to make a million more first times
-(MM, mm)
-The greatest thing that I have achieved
-Was four little words, down on one knee
-You said, "Darling, are you jokin'? ", and I just said, "Please"
-Ain't it funny how the simplest things in life can make a man?
-Little moments that pass us by
-Oh, but I remember
-The first kiss, the first night, the first song that made you cry
-The first look in your eyes when I said "I love you", I
-Can still feel the butterflies from when we stumbled home that night
-I can't wait to make a million more first times
-(MM, mm)
-Ain't it funny how the simplest things in life can make a man?
-Little moments that pass us by
-Oh, but I remember
-The first kiss, first night, first song that made you cry
-First dance in moonlight in your parents' garden, I
-Can't wait to see everything that's yet to be
-Our first child and then a million more first times</t>
-  </si>
-  <si>
-    <t>One, two, three, four
-Ooh-ooh, ooh-ooh-ooh
-Every time you come around, you know I can't say no
-Every time the sun goes down, I let you take control
-I can feel the paradise before my world implodes
-And tonight had something wonderful
-My bad habits lead to late nights endin' alone
-Conversations with a stranger I barely know
-Swearin' this will be the last, but it probably won't
-I got nothin' left to lose, or use, or do
-My bad habits lead to wide eyes stare into space
-And I know I'll lose control of the things that I say
-Yeah, I was lookin' for a way out, now I can't escape
-Nothin' happens after two, it's true
-It's true, my bad habits lead to you
-Ooh-ooh, ooh-ooh-ooh
-My bad habits lead to you
-Ooh-ooh, ooh-ooh-ooh
-My bad habits lead to you
-Every pure intention ends when the good times start
-Fallin' over everything to reach the first time's spark
-It started under neon lights, and then it all got dark
-I only know how to go too far
-My bad habits lead to late nights endin' alone
-Conversations with a stranger I barely know
-Swearin' this will be the last, but it probably won't
-I got nothin' left to lose, or use, or do
-My bad habits lead to wide eyes stare into space
-And I know I'll lose control of the things that I say
-Yeah, I was lookin' for a way out, now I can't escape
-Nothin' happens after two, it's true
-It's true, my bad habits lead to you
-Ooh-ooh, ooh-ooh-ooh
-My bad habits lead to you
-Ooh-ooh, ooh-ooh-ooh
-We took the long way 'round
-And burned 'til the fun ran out, now
-My bad habits lead to late nights endin' alone
-Conversations with a stranger I barely know
-Swearin' this will be the last, but it probably won't
-I got nothin' left to lose, or use, or do
-My bad habits lead to wide eyes stare into space
-And I know I'll lose control of the things that I say
-Yeah, I was lookin' for a way out, now I can't escape
-Nothin' happens after two, it's true
-It's true, my bad habits lead to you
-Ooh-ooh, ooh-ooh-ooh
-My bad habits lead to you
-Ooh-ooh, ooh-ooh-ooh
-My bad habits lead to you</t>
+    <t>I have grown up I am a father now Everything has changed but I am still the same somehow You know I've never been afraid of death But now I wanna see the things that haven't happened yet I still love getting out of my mind I should cut it down I still know people I don't like and I should cut them out I feel embarrassed 'bout the things that I did in my youth 'Cause now I have a child I know one day that you will do it Freight cargo dot stops and aeroplanes Late-night calls signal is in and out again Feelin' low serotonin known better days Go go go! But every moment you're here with me Timе stops to still When you are in my arms it always will And life lifе is changin' tides I lost the confidence in who I was Too busy tryna chase the high and get the numbers up I have the same dream every night A bullet through my brain the moment that I close my eyes I still have to lean on a shoulder when I've broken down And I have people that depend on me to sort them out I sometimes fantasize I disappear without a trace I've no regrets but wish I did things in a different way Low fly zone lawsuits and film stars Headline wrote the princess and the face scar Broken bones break-ins and Babylon Go go go! But every moment you're here with me Time stops to still When you are in my arms it always will And life life is changin' tides Time stops to still When you are in my arms it always will And life life is changin' tides</t>
+  </si>
+  <si>
+    <t>I took an arrow to the heart I never kissed a mouth that tastes like yours Strawberries and somethin' more Ooh yeah I want it all Lipstick on my guitar (ooh) Fill up the engine we can drive real far Go dancin' underneath the stars Ooh yeah I want it all Mm you got me feelin' like I wanna be that guy I wanna kiss your eyes I wanna drink that smile I wanna feel like I'm Like my soul's on fire I wanna stay up all day and all night Yeah you got me singin' like Ooh I love it when you do it like that And when you're close up give me the shivers Oh baby you wanna dance 'til the sunlight cracks And when they say the party's over then we'll bring it right back And we'll say ooh I love it when you do it like that And when you're close up give me the shivers Oh baby you wanna dance 'til the sunlight cracksAnd when they say the party's over then we'll bring it right back Into the car On the backseat in the moonlit dark Wrap me up between your legs and arms Ooh I can't get enough You know you could tear me apart (ooh) Put me back together and take my heart I never thought that I could love this hard Ooh I can't get enough Mm you got me feeling like I wanna be that guy I wanna kiss your eyes I wanna drink that smile I wanna feel like I'm Like my soul's on fire I wanna stay up all day and all night Yeah you got me singin' like Ooh I love it when you do it like that And when you're close up give me the shivers Oh baby you wanna dance 'til the sunlight cracks And when they say the party's over then we'll bring it right back And we'll say ooh I love it when you do it like that And when you're close up give me the shivers Oh baby you wanna dance 'til the sunlight cracks And when they say the party's over then we'll bring it right back Baby you burn so hot You make me shiver with the fire you got This thing we started I don't want it to stop You know you make me shiver-er-er Baby you burn so hot You make me shiver with the fire you got This thing we started I don't want it to stop You know you make me shiver Yeah you got me singin' like Ooh I love it when you do it like that And when you're close up give me the shivers Oh baby you wanna dance 'til the sunlight cracks And when they say the party's over then we'll bring it right back (oh no) And we'll say ooh I love it when you do it like that And when you're close up give me the shivers Oh baby you wanna dance 'til the sunlight cracks And when they say the party's over then we'll bring it right back hey</t>
+  </si>
+  <si>
+    <t>I thought it'd feel different playin' Wembley
+ Eighty thousand singin' with me
+ It's what I've been chasin' 'cause this is the dream
+ When it was all over I cleared out the room
+ Grabbed a couple beers just me and you
+ Then we started talking the way that we do
+ Ain't it funny how the simplest things in life can make a man?
+ Little moments that pass us by
+ Oh but I remember
+ The first kiss the first night the first song that made you cry
+ The first drink red wine on a step in Brooklyn I
+ Still feel the first fight and we both made it out alive
+ And I can't wait to make a million more first times
+ (MM mm)
+ The greatest thing that I have achieved
+ Was four little words down on one knee
+ You said "Darling are you jokin'? " and I just said "Please"
+ Ain't it funny how the simplest things in life can make a man?
+ Little moments that pass us by
+ Oh but I remember
+ The first kiss the first night the first song that made you cry
+ The first look in your eyes when I said "I love you" I
+ Can still feel the butterflies from when we stumbled home that night
+ I can't wait to make a million more first times
+ (MM mm)
+ Ain't it funny how the simplest things in life can make a man?
+ Little moments that pass us by
+ Oh but I remember
+ The first kiss first night first song that made you cry
+ First dance in moonlight in your parents' garden I
+ Can't wait to see everything that's yet to be
+ Our first child and then a million more first times</t>
+  </si>
+  <si>
+    <t>One two three four
+ Ooh-ooh ooh-ooh-ooh
+ Every time you come around you know I can't say no
+ Every time the sun goes down I let you take control
+ I can feel the paradise before my world implodes
+ And tonight had something wonderful
+ My bad habits lead to late nights endin' alone
+ Conversations with a stranger I barely know
+ Swearin' this will be the last but it probably won't
+ I got nothin' left to lose or use or do
+ My bad habits lead to wide eyes stare into space
+ And I know I'll lose control of the things that I say
+ Yeah I was lookin' for a way out now I can't escape
+ Nothin' happens after two it's true
+ It's true my bad habits lead to you
+ Ooh-ooh ooh-ooh-ooh
+ My bad habits lead to you
+ Ooh-ooh ooh-ooh-ooh
+ My bad habits lead to you
+ Every pure intention ends when the good times start
+ Fallin' over everything to reach the first time's spark
+ It started under neon lights and then it all got dark
+ I only know how to go too far
+ My bad habits lead to late nights endin' alone
+ Conversations with a stranger I barely know
+ Swearin' this will be the last but it probably won't
+ I got nothin' left to lose or use or do
+ My bad habits lead to wide eyes stare into space
+ And I know I'll lose control of the things that I say
+ Yeah I was lookin' for a way out now I can't escape
+ Nothin' happens after two it's true
+ It's true my bad habits lead to you
+ Ooh-ooh ooh-ooh-ooh
+ My bad habits lead to you
+ Ooh-ooh ooh-ooh-ooh
+ We took the long way 'round
+ And burned 'til the fun ran out now
+ My bad habits lead to late nights endin' alone
+ Conversations with a stranger I barely know
+ Swearin' this will be the last but it probably won't
+ I got nothin' left to lose or use or do
+ My bad habits lead to wide eyes stare into space
+ And I know I'll lose control of the things that I say
+ Yeah I was lookin' for a way out now I can't escape
+ Nothin' happens after two it's true
+ It's true my bad habits lead to you
+ Ooh-ooh ooh-ooh-ooh
+ My bad habits lead to you
+ Ooh-ooh ooh-ooh-ooh
+ My bad habits lead to you</t>
   </si>
   <si>
     <t>This is a dark parade
-Another rough patch to rain on, to rain on
+Another rough patch to rain on to rain on
 I know your friends may say
-This is a cause for celebration, hip-hip-hooray, love
+This is a cause for celebration hip-hip-hooray love
 Photographs in sepia tones
-It's so still, the fire's barely fighting the cold, alone
+It's so still the fire's barely fighting the cold alone
 There are times when I can feel your ghost
 Just when I'm almost letting you go
 The cards were stacked against us both
 I will always love you for what it's worth
 We'll never fade like graffiti on the overpass
 And I know time may change the way you think of us
-But I'll remember the way we were, you were the first full stop
+But I'll remember the way we were you were the first full stop
 Love that will never leave
-Baby, you will never be lost on me
+Baby you will never be lost on me
 This is a goddamn shame
-I never wanted to break it, or leave us tainted
+I never wanted to break it or leave us tainted
 Know I should walk away
-But I just can't replace us, or even erase us
-The car was stuck, the engine stalled
-And both of us got caught out in the snow, alone
+But I just can't replace us or even erase us
+The car was stuck the engine stalled
+And both of us got caught out in the snow alone
 There were times when I forget the lows
 And think the highs were all that we'd ever known
 The cards were stacked against us both
 I will always love you for what it's worth
 We'll never fade like graffiti on the overpass
 And I know time may change the way you think of us
-But I'll remember the way we were, you were the first full stop
+But I'll remember the way we were you were the first full stop
 Love that will never leave
-Baby, you will never be lost on me
+Baby you will never be lost on me
 Lost on me
-Baby, you will never be lost on me
+Baby you will never be lost on me
 Lost on me
-Well, I will always love you for what it's worth
+Well I will always love you for what it's worth
 We'll never fade like graffiti on the overpass
 And I know time may change the way you think of us
-But I'll remember the way we were, you were the first full stop
+But I'll remember the way we were you were the first full stop
 Love that will never leave
-Baby, you will never be lost on me
-Yeah, yeah, yeah
-Yeah, yeah, yeah
+Baby you will never be lost on me
+Yeah yeah yeah
+Yeah yeah yeah
 Lost on me
-Ooh, graffiti on the overpass</t>
+Ooh graffiti on the overpass</t>
   </si>
   <si>
     <t>How was I to know? It's a crazy thing
-I showed you my hand and you still let me win
-And who was I to say that this was meant to be?
-The road that was broken brought us together
-And I know you could fall for a thousand kings
-And hearts that would give you a diamond ring
-When I fold, you see the best in me
-The joker and the queen
-I was upside down from the outside in
-You came to the table and you went all in
-With a single word and a gentle touch
-You turned a moment into forever
-And I know you could fall for a thousand kings
-And hearts that could give you a diamond ring
-When I fold, you see the best in me
-The joker and the queen
-And I know you could fall for a thousand kings
-And hearts that would givе you a diamond ring
-When I folded, you saw the bеst in me
-The joker and the queen
-The joker and the queen</t>
+ I showed you my hand and you still let me win
+ And who was I to say that this was meant to be?
+ The road that was broken brought us together
+ And I know you could fall for a thousand kings
+ And hearts that would give you a diamond ring
+ When I fold you see the best in me
+ The joker and the queen
+ I was upside down from the outside in
+ You came to the table and you went all in
+ With a single word and a gentle touch
+ You turned a moment into forever
+ And I know you could fall for a thousand kings
+ And hearts that could give you a diamond ring
+ When I fold you see the best in me
+ The joker and the queen
+ And I know you could fall for a thousand kings
+ And hearts that would givе you a diamond ring
+ When I folded you saw the bеst in me
+ The joker and the queen
+ The joker and the queen</t>
   </si>
   <si>
     <t>If I forget to say goodbye
-Before I catch the plane
-Would you know the way that I
-Feel when I'm away?
-We'll see the same sky tonight
-But the stars are out of place
-You'll never know the weight of my heart
-Every time I leave you, babe
-It's hard to break the landing
-But I'll see you again
-I'm never gonna leave your life
-Even at the times I'm miles away
-You are always on my mind
-Forever and now, I will be by your side
-I know it can change from day to day
-But this love will keep alive
-I'm never gonna leave your life
-I-I-I'm, I'm never gonna leave your life
-Oh, I could never tell you lie
-Or put in words your finest traits
-The darkest green and hazel eyes
-And yet I can't describe the shade
-You are all this heart of mine
-And there you will remain
-You'll never know the weight of my
-Decisions when I leave your smiling face
-It's hard to understand it
-But I'll see you again
-Oh, I'm, I'm never gonna leave your life
-Even at the times I'm miles away
-You are always on my mind
-Forever and now, I will be by your side
-I know it can change from day to day
-But this love will keep alive
-I'm never gonna leave your life
-I-I-I'm, I'm never gonna leave your life
-It's hard to break the landing
-But I'll see you again
-I'm never gonna leave your life
-Even at the times I'm miles away
-You are always on my mind
-Forever and now, I will be by your side
-I know it can change from day to day
-But this love will keep alive
-I'm never gonna leave your life
-I-I I'm, I'm never gonna leave your life
-If I forget to say goodbye
-Before I catch the plane
-Would you know the way that I
-Feel when I'm away?</t>
-  </si>
-  <si>
-    <t>Oh yeah, we've been in the rain
-Been on the rocks, but we found our way
-We've ordered pizza to an aeroplane
-Slept on the beach like we were castaways
-We've been in the storm
-Been to an Irish bar in central Rome
-Driven to hospitals with broken bones
-We've shared a toothbrush and shared our home
-We've seen the moon reflect on the rollin' tide
-Been up at 5AM, watchin' the sunrise
-Becausе the world looks better whеn I'm by your side
-Oh I, oh I, oh I
-When you and I collide
-You bring me to life
-Yeah, you bring me to life
-You bring me to life
-When you and I collide
-You bring me to life
-Yeah, you bring me to life
-You bring me to life
-We've been on the road
-We've watched the blossom fall to Earth like snow
-Fumbled in cubicles in Tokyo
-And been to funerals in rented clothes
-MM, we drank your father's whiskey
-When your grandma died
-You brought me to the morning through my darkest night
-Yeah the world hurts less when I'm by your side
-Oh I, oh I, oh I
-When you and I collide
-You bring me to life
-Yeah, you bring me to life
-You bring me to life
-When you and I collide
-You bring me to life
-Yeah, you bring me to life
-You bring me to life
-Head first, collidin'
-Dreamers collidin'
-Universe collidin'
-Your love let the light in
-Head first, collidin'
-Dreamers collidin'
-Universe collidin'
-We made love in the sky
-Overslept and missed the Northern Lights
-You lost your wedding ring, but I didn't mind
-‘Cause I got a feeling, baby, we'll be fine</t>
+ Before I catch the plane
+ Would you know the way that I
+ Feel when I'm away?
+ We'll see the same sky tonight
+ But the stars are out of place
+ You'll never know the weight of my heart
+ Every time I leave you babe
+ It's hard to break the landing
+ But I'll see you again
+ I'm never gonna leave your life
+ Even at the times I'm miles away
+ You are always on my mind
+ Forever and now I will be by your side
+ I know it can change from day to day
+ But this love will keep alive
+ I'm never gonna leave your life
+ I-I-I'm I'm never gonna leave your life
+ Oh I could never tell you lie
+ Or put in words your finest traits
+ The darkest green and hazel eyes
+ And yet I can't describe the shade
+ You are all this heart of mine
+ And there you will remain
+ You'll never know the weight of my
+ Decisions when I leave your smiling face
+ It's hard to understand it
+ But I'll see you again
+ Oh I'm I'm never gonna leave your life
+ Even at the times I'm miles away
+ You are always on my mind
+ Forever and now I will be by your side
+ I know it can change from day to day
+ But this love will keep alive
+ I'm never gonna leave your life
+ I-I-I'm I'm never gonna leave your life
+ It's hard to break the landing
+ But I'll see you again
+ I'm never gonna leave your life
+ Even at the times I'm miles away
+ You are always on my mind
+ Forever and now I will be by your side
+ I know it can change from day to day
+ But this love will keep alive
+ I'm never gonna leave your life
+ I-I I'm I'm never gonna leave your life
+ If I forget to say goodbye
+ Before I catch the plane
+ Would you know the way that I
+ Feel when I'm away?</t>
+  </si>
+  <si>
+    <t>Oh yeah we've been in the rain
+ Been on the rocks but we found our way
+ We've ordered pizza to an aeroplane
+ Slept on the beach like we were castaways
+ We've been in the storm
+ Been to an Irish bar in central Rome
+ Driven to hospitals with broken bones
+ We've shared a toothbrush and shared our home
+ We've seen the moon reflect on the rollin' tide
+ Been up at 5AM watchin' the sunrise
+ Becausе the world looks better whеn I'm by your side
+ Oh I oh I oh I
+ When you and I collide
+ You bring me to life
+ Yeah you bring me to life
+ You bring me to life
+ When you and I collide
+ You bring me to life
+ Yeah you bring me to life
+ You bring me to life
+ We've been on the road
+ We've watched the blossom fall to Earth like snow
+ Fumbled in cubicles in Tokyo
+ And been to funerals in rented clothes
+ MM we drank your father's whiskey
+ When your grandma died
+ You brought me to the morning through my darkest night
+ Yeah the world hurts less when I'm by your side
+ Oh I oh I oh I
+ When you and I collide
+ You bring me to life
+ Yeah you bring me to life
+ You bring me to life
+ When you and I collide
+ You bring me to life
+ Yeah you bring me to life
+ You bring me to life
+ Head first collidin'
+ Dreamers collidin'
+ Universe collidin'
+ Your love let the light in
+ Head first collidin'
+ Dreamers collidin'
+ Universe collidin'
+ We made love in the sky
+ Overslept and missed the Northern Lights
+ You lost your wedding ring but I didn't mind
+ ‘Cause I got a feeling baby we'll be fine</t>
   </si>
   <si>
     <t>I had a bad week
-Spent the evening pretending it wasn't that deep
-You could see in my eyes that it was taking over
-I guess I was just blind and caught up in the moment
-You know you take all of my stress right down
-Help me get it off my chest and out
-Into the ether with the rest of this mess
-That just keeps us depressed
-We forget that we're here right now
-'Cause we're livin' life at a different pace
-Stuck in a constant race
-Keep the pressure on, you're bound to break
-Something's got to change
-We should just be cancelling all our plans
-And not give a damn
-If we're missin' out on what the people think is right
-Seein' through a picture behind the screen and forget to be
-Lose the conversation for the message that you'll never read
-I think maybe you and me
-Oh, we should head out to the place where the music plays
-And then
-We'll go all night
-Two-steppin' with the woman I love
-All my troubles turn to nothin'
-When I'm in your eyes, electrified
-We'll keep turnin' up and go all night
-Oh, we had dips and falls in our time
-But we know what it feels to be low, then up
-Alone, then loved
-And all we need is us to go all
-Night, night
-Two-steppin' with the woman I love
-Night, yeah
-All we need is us
-What do you reckon, is it just me?
-Words are weapons and occasionally they cut deep
-Crisis of confidence, it tends to come
-When I feel the dark and I open my heart
-If you don't see it, you should trust me
-I feel like I got nothin' left right now
-Except this beauty in her dress right now
-She got me feelin' like the best
-And the rest are just less than she needs
-So we press play and step to the beat
-'Cause we're livin' life at a different pace
-Stuck in a constant race
-Keep the pressure on, you're bound to break
-Something's got to change
-We should just be cancelling all our plans
-And not give a damn
-Head out to the place where it plays and
-We'll go all night
-Two-steppin' with the woman I love
-All my troubles turn to nothin'
-When I'm in your eyes, electrified
-We'll keep turnin' up and go all night
-Oh, we had dips and falls in our time
-But we know what it feels to be low, then up
-Alone and loved
-And all we need is us to go all
-Night, night
-Two-steppin' with the woman I love
-Night, yeah
-All we need is us to go all night
-Night, night
-Two-steppin' with the woman I love
-Night, yeah
-All we need is us to go all night</t>
+ Spent the evening pretending it wasn't that deep
+ You could see in my eyes that it was taking over
+ I guess I was just blind and caught up in the moment
+ You know you take all of my stress right down
+ Help me get it off my chest and out
+ Into the ether with the rest of this mess
+ That just keeps us depressed
+ We forget that we're here right now
+ 'Cause we're livin' life at a different pace
+ Stuck in a constant race
+ Keep the pressure on you're bound to break
+ Something's got to change
+ We should just be cancelling all our plans
+ And not give a damn
+ If we're missin' out on what the people think is right
+ Seein' through a picture behind the screen and forget to be
+ Lose the conversation for the message that you'll never read
+ I think maybe you and me
+ Oh we should head out to the place where the music plays
+ And then
+ We'll go all night
+ Two-steppin' with the woman I love
+ All my troubles turn to nothin'
+ When I'm in your eyes electrified
+ We'll keep turnin' up and go all night
+ Oh we had dips and falls in our time
+ But we know what it feels to be low then up
+ Alone then loved
+ And all we need is us to go all
+ Night night
+ Two-steppin' with the woman I love
+ Night yeah
+ All we need is us
+ What do you reckon is it just me?
+ Words are weapons and occasionally they cut deep
+ Crisis of confidence it tends to come
+ When I feel the dark and I open my heart
+ If you don't see it you should trust me
+ I feel like I got nothin' left right now
+ Except this beauty in her dress right now
+ She got me feelin' like the best
+ And the rest are just less than she needs
+ So we press play and step to the beat
+ 'Cause we're livin' life at a different pace
+ Stuck in a constant race
+ Keep the pressure on you're bound to break
+ Something's got to change
+ We should just be cancelling all our plans
+ And not give a damn
+ Head out to the place where it plays and
+ We'll go all night
+ Two-steppin' with the woman I love
+ All my troubles turn to nothin'
+ When I'm in your eyes electrified
+ We'll keep turnin' up and go all night
+ Oh we had dips and falls in our time
+ But we know what it feels to be low then up
+ Alone and loved
+ And all we need is us to go all
+ Night night
+ Two-steppin' with the woman I love
+ Night yeah
+ All we need is us to go all night
+ Night night
+ Two-steppin' with the woman I love
+ Night yeah
+ All we need is us to go all night</t>
   </si>
   <si>
     <t>Another human cloud to bring you down when you blew the last away
-And bring out a poisoned tongue or plastic crown, but for me, they look the same
-Sometimes, it can get all too much for me
-And that's why the photograph gets burned, throw the match in gasoline, a-ayy
-Don't let the ones who hurt you see you cry
-Tomorrow is another day
-You cannot stop the rain, no way
-Holdin' an umbrella when the rain clouds come over again
-Tryna find somethin' real, but it's not the game they play
-Pretending that the weather is in your mind, you got no one to blame
-But that's just the way I feel
-You cannot stop the rain, yeah, yeah, yeah, yeah
-You cannot stop the rain, yeah, yeah, yeah, yeah
-Another "I, me, mine" to blur the lines between love and then heartbreak
-Oh, it's a lonely life thinkin' you're right and always shiftin' blame
-And every time it's getting more and more ugly
-And that's why the photograph gets burned, throw the match in gasoline, a-ayy
-Don't let them tell you "Keep it all inside"
-I know the winds have got to change
-You cannot stop the rain, no way
-Holdin' an umbrella when the rain clouds come over again
-Tryna find somethin' real, but it's not the game they play
-Pretending that the weather is in your mind, you got no one to blame
-But that's just the way I feel
-You cannot stop the rain, yeah, yeah, yeah, yeah
-You cannot stop the rain, yeah, yeah, yeah, yeah
-And it seem like time
-Can be so much more than a wake-up call into live real life
-Every day is a chance that we can start over, read my mind
-There'll be ups and downs, but it won't change a thing between you and I
-There's one thing I can't change
-You cannot stop the rain, no way
-Holdin' an umbrella when the rain clouds come over again
-Tryna find somethin' real, but it's not the game they play
-Pretending that the weather is in your mind, you got no one to blame
-But that's just the way I feel
-You cannot stop the rain, no way
-Holdin' an umbrella when the rain clouds come over again
-Tryna find somethin' real, but it's not the game they play
-Pretending that the weather is in your mind, you got no one to blame
-But that's just the way I feel
-You cannot stop the rain, yeah, yeah, yeah, yeah
-You cannot stop the rain, yeah, yeah, yeah, yeah
-Can't stop the rain, yeah, can't stop the rain, yeah (Yeah, yeah, yeah, yeah)
-Can't stop the rain, can't stop the rain (Yeah, yeah, yeah, yeah)
-Can't stop the rain (Yeah, yeah, yeah, yeah)
-You know you can't stop the rain, yeah, yeah, yeah, yeah</t>
+ And bring out a poisoned tongue or plastic crown but for me they look the same
+ Sometimes it can get all too much for me
+ And that's why the photograph gets burned throw the match in gasoline a-ayy
+ Don't let the ones who hurt you see you cry
+ Tomorrow is another day
+ You cannot stop the rain no way
+ Holdin' an umbrella when the rain clouds come over again
+ Tryna find somethin' real but it's not the game they play
+ Pretending that the weather is in your mind you got no one to blame
+ But that's just the way I feel
+ You cannot stop the rain yeah yeah yeah yeah
+ You cannot stop the rain yeah yeah yeah yeah
+ Another "I me mine" to blur the lines between love and then heartbreak
+ Oh it's a lonely life thinkin' you're right and always shiftin' blame
+ And every time it's getting more and more ugly
+ And that's why the photograph gets burned throw the match in gasoline a-ayy
+ Don't let them tell you "Keep it all inside"
+ I know the winds have got to change
+ You cannot stop the rain no way
+ Holdin' an umbrella when the rain clouds come over again
+ Tryna find somethin' real but it's not the game they play
+ Pretending that the weather is in your mind you got no one to blame
+ But that's just the way I feel
+ You cannot stop the rain yeah yeah yeah yeah
+ You cannot stop the rain yeah yeah yeah yeah
+ And it seem like time
+ Can be so much more than a wake-up call into live real life
+ Every day is a chance that we can start over read my mind
+ There'll be ups and downs but it won't change a thing between you and I
+ There's one thing I can't change
+ You cannot stop the rain no way
+ Holdin' an umbrella when the rain clouds come over again
+ Tryna find somethin' real but it's not the game they play
+ Pretending that the weather is in your mind you got no one to blame
+ But that's just the way I feel
+ You cannot stop the rain no way
+ Holdin' an umbrella when the rain clouds come over again
+ Tryna find somethin' real but it's not the game they play
+ Pretending that the weather is in your mind you got no one to blame
+ But that's just the way I feel
+ You cannot stop the rain yeah yeah yeah yeah
+ You cannot stop the rain yeah yeah yeah yeah
+ Can't stop the rain yeah can't stop the rain yeah (Yeah yeah yeah yeah)
+ Can't stop the rain can't stop the rain (Yeah yeah yeah yeah)
+ Can't stop the rain (Yeah yeah yeah yeah)
+ You know you can't stop the rain yeah yeah yeah yeah</t>
   </si>
   <si>
     <t>It's been a while since we've been alone
-To turn off the world and the telephone
-I need to tell you you're beautiful
-'Cause it's been a while and I apologize
-I just get caught up in the rat race I'm runnin'
-Chasin' a moment, I'm hoping is comin'
-If I stopped and took a look around
-It's in front of my eyes, eyes
-Baby, let's slow down time
-Maybe just press rewind
-Darling, that dress reminds
-Me of the first time
-And I wanna love tonight
-One on one by the candlelight
-Over and over, we spend our lives
-Living fast forward but not tonight
-Love in slow motion
-It's been a while since it was you and me
-Too many friends, too many evening drinks
-Yeah, we commit to so many things
-But not to ourselves, and I apologize
-Sometimes you're sad and you tell me it's nothin'
-And I brush it off because there's always somethin'
-But I need to change my perspective
-And prioritize-ize
-If there's one thing I know, it's this
-Every moment missed
-Can be restored with your lips
-It only takes one kiss
-And I wanna love tonight
-One on one by the candlelight
-Over and over, we spend our lives
-Living fast forward but not tonight
-Love in slow motion
-Ooh-ooh
-Ooh-ooh
-Love tonight
-One on one by the candlelight
-Over and over, we spend our lives
-Living fast forward but not tonight
-Love in slow motion
-Wanna love tonight
-One on one by the candlelight
-Over and over, we spend our lives
-Living fast forward but not tonight
-Love in slow motion
-In slow motion
-In slow motion</t>
+ To turn off the world and the telephone
+ I need to tell you you're beautiful
+ 'Cause it's been a while and I apologize
+ I just get caught up in the rat race I'm runnin'
+ Chasin' a moment I'm hoping is comin'
+ If I stopped and took a look around
+ It's in front of my eyes eyes
+ Baby let's slow down time
+ Maybe just press rewind
+ Darling that dress reminds
+ Me of the first time
+ And I wanna love tonight
+ One on one by the candlelight
+ Over and over we spend our lives
+ Living fast forward but not tonight
+ Love in slow motion
+ It's been a while since it was you and me
+ Too many friends too many evening drinks
+ Yeah we commit to so many things
+ But not to ourselves and I apologize
+ Sometimes you're sad and you tell me it's nothin'
+ And I brush it off because there's always somethin'
+ But I need to change my perspective
+ And prioritize-ize
+ If there's one thing I know it's this
+ Every moment missed
+ Can be restored with your lips
+ It only takes one kiss
+ And I wanna love tonight
+ One on one by the candlelight
+ Over and over we spend our lives
+ Living fast forward but not tonight
+ Love in slow motion
+ Ooh-ooh
+ Ooh-ooh
+ Love tonight
+ One on one by the candlelight
+ Over and over we spend our lives
+ Living fast forward but not tonight
+ Love in slow motion
+ Wanna love tonight
+ One on one by the candlelight
+ Over and over we spend our lives
+ Living fast forward but not tonight
+ Love in slow motion
+ In slow motion
+ In slow motion</t>
   </si>
   <si>
     <t>I wish that heaven
-Had visiting hours
-So I could just show up
-And bring the news
-That she's getting older
-And I wish that you'd met her
-The things that she'll learn from me
-I got them all from you
-Can I just stay a while and we'll put all the world to rights?
-The little ones will grow and I'll still drink your favourite wine
-And soon, they're going to close, but I'll see you another day
-So much has changed since you've been away
-Well, I wish that heaven
-Had visiting hours
-So I could just swing by
-And ask your advice
-What would you do in my situation?
-I haven't a clue how I'd even raise them
-What would you do?
-'Cause you always do what's right
-Can we just talk a while until my worries disappear?
-I'd tell you that I'm scared of turning out a failure
-You'd say, "Remember that the answer's
-In the love that we create"
-So much has changed since you've been away
-I wish that heaven
-Had visiting hours
-And I would ask them
-If I could take you home
-But I know what they'd say
-That it's for the best
-So I would live life the way you told me
-And make it on my own
-And I will close the door, but I will open up my heart
-And everyone I love will know exactly who you are
-'Cause this is not goodbye, it is just 'til we meet again
-So much has changed since you've been away</t>
+ Had visiting hours
+ So I could just show up
+ And bring the news
+ That she's getting older
+ And I wish that you'd met her
+ The things that she'll learn from me
+ I got them all from you
+ Can I just stay a while and we'll put all the world to rights?
+ The little ones will grow and I'll still drink your favourite wine
+ And soon they're going to close but I'll see you another day
+ So much has changed since you've been away
+ Well I wish that heaven
+ Had visiting hours
+ So I could just swing by
+ And ask your advice
+ What would you do in my situation?
+ I haven't a clue how I'd even raise them
+ What would you do?
+ 'Cause you always do what's right
+ Can we just talk a while until my worries disappear?
+ I'd tell you that I'm scared of turning out a failure
+ You'd say "Remember that the answer's
+ In the love that we create"
+ So much has changed since you've been away
+ I wish that heaven
+ Had visiting hours
+ And I would ask them
+ If I could take you home
+ But I know what they'd say
+ That it's for the best
+ So I would live life the way you told me
+ And make it on my own
+ And I will close the door but I will open up my heart
+ And everyone I love will know exactly who you are
+ 'Cause this is not goodbye it is just 'til we meet again
+ So much has changed since you've been away</t>
   </si>
   <si>
     <t>You were loved before you had arrived
-And every day that love just multiplies
-Daddy made your bed and your lullaby
-And Mumma made the mobile in the sky
-And loving you is easy
-But life will not always be
-Fall into the world of your song
-Whatever you feel can never be wrong
-Come along for the ride
-And in the shake of a lamb's tail, we'll go
-Yeah, be still now and close your eyes
-And dream
-Hanging out with the sandman
-You look so sweet, my child
-Hanging out with the sandman
-And though there's rain outside, you'll bе warm and dry
-The thunder and the lightning won't hurt you now
-So go to sleep, my lovе
-Hanging out with the sandman
-Chocolate-covered roof and candy cars
-Rainbow sugar river we can sail upon
-Marshmallow books and strawberries
-Snowmen made of ice cream
-Over the flower fields, we'll fly
-We'll count the fish in the sky
-Honeybees and birds sing your song
-Whatever you feel can never be wrong
-Come along for the ride
-And in the shake of a lamb's tail, we'll go
-Yeah, be still now and close your eyes
-And dream
-Hanging out with the sandman
-You look so sweet, my child
-Hanging out with the sandman
-And though there's rain outside, you'll be warm and dry
-The thunder and the lightning won't hurt you now
-So go to sleep, my love
-Hanging out with the sandman
-Come along for the ride
-And in the shake of a lamb's tail, we'll go
-Yeah, be still now and close your eyes
-And dream
-Hanging out with the sandman
-You look so sweet, my child
-Hanging out with the sandman
-And though there's rain outside, you'll be warm and dry
-The thunder and the lightning won't hurt you now
-So go to sleep, my love
-Hanging out with the sandman
-We're hanging out with the sandman
-We're hanging out with the sandman
-We're hanging out with the sandman</t>
+ And every day that love just multiplies
+ Daddy made your bed and your lullaby
+ And Mumma made the mobile in the sky
+ And loving you is easy
+ But life will not always be
+ Fall into the world of your song
+ Whatever you feel can never be wrong
+ Come along for the ride
+ And in the shake of a lamb's tail we'll go
+ Yeah be still now and close your eyes
+ And dream
+ Hanging out with the sandman
+ You look so sweet my child
+ Hanging out with the sandman
+ And though there's rain outside you'll bе warm and dry
+ The thunder and the lightning won't hurt you now
+ So go to sleep my lovе
+ Hanging out with the sandman
+ Chocolate-covered roof and candy cars
+ Rainbow sugar river we can sail upon
+ Marshmallow books and strawberries
+ Snowmen made of ice cream
+ Over the flower fields we'll fly
+ We'll count the fish in the sky
+ Honeybees and birds sing your song
+ Whatever you feel can never be wrong
+ Come along for the ride
+ And in the shake of a lamb's tail we'll go
+ Yeah be still now and close your eyes
+ And dream
+ Hanging out with the sandman
+ You look so sweet my child
+ Hanging out with the sandman
+ And though there's rain outside you'll be warm and dry
+ The thunder and the lightning won't hurt you now
+ So go to sleep my love
+ Hanging out with the sandman
+ Come along for the ride
+ And in the shake of a lamb's tail we'll go
+ Yeah be still now and close your eyes
+ And dream
+ Hanging out with the sandman
+ You look so sweet my child
+ Hanging out with the sandman
+ And though there's rain outside you'll be warm and dry
+ The thunder and the lightning won't hurt you now
+ So go to sleep my love
+ Hanging out with the sandman
+ We're hanging out with the sandman
+ We're hanging out with the sandman
+ We're hanging out with the sandman</t>
   </si>
   <si>
     <t>A lifetime startin' to feel like
-It's fallin' short of the mark
-But it's all that we got
-Every teardrop, every wrong turn
-Made the moment we found
-And it's comin' around, around, around, around, around
-I don't wanna miss one thing
-We can turn the whole world down
-And listen to the in-between
-We are, we are the sound
-There's nothin' but the space we're in
-The hurry and the noise shut out
-Just stay here and be right now
-The shadows cling to the ceiling
-And fracture the light
-That lands in our eyes
-Every moment changes the whole view
-And just when it ends
-I feel it again, again, again, again, again
-I don't wanna miss one thing
-We can turn the whole world down
-And listen to the in-between
-We are, we are the sound
-There's nothin' but the space we're in
-The hurry and the noise shut out
-Just stay here and be right now
-Nothing else matters
-Nothing else matters
-Nothing else matters
-Stay here and be right now
-Nothing else matters
-Nothing else matters
-Nothing else matters
-Just stay here and be right now
-I don't wanna miss one thing
-We can turn the whole world down
-And listen to the in-between
-We are, we are the sound
-There's nothing but the space we're in
-The hurry and the noise shut out
-Just stay here and be right now</t>
+ It's fallin' short of the mark
+ But it's all that we got
+ Every teardrop every wrong turn
+ Made the moment we found
+ And it's comin' around around around around around
+ I don't wanna miss one thing
+ We can turn the whole world down
+ And listen to the in-between
+ We are we are the sound
+ There's nothin' but the space we're in
+ The hurry and the noise shut out
+ Just stay here and be right now
+ The shadows cling to the ceiling
+ And fracture the light
+ That lands in our eyes
+ Every moment changes the whole view
+ And just when it ends
+ I feel it again again again again again
+ I don't wanna miss one thing
+ We can turn the whole world down
+ And listen to the in-between
+ We are we are the sound
+ There's nothin' but the space we're in
+ The hurry and the noise shut out
+ Just stay here and be right now
+ Nothing else matters
+ Nothing else matters
+ Nothing else matters
+ Stay here and be right now
+ Nothing else matters
+ Nothing else matters
+ Nothing else matters
+ Just stay here and be right now
+ I don't wanna miss one thing
+ We can turn the whole world down
+ And listen to the in-between
+ We are we are the sound
+ There's nothing but the space we're in
+ The hurry and the noise shut out
+ Just stay here and be right now</t>
+  </si>
+  <si>
+    <t>It's such a beautiful night
+ To make a change in our lives
+ East Anglian sky empty bottle of wine
+ I got you by my side talkin'
+ About love and life
+ Oh how lucky am I when I look in your eyes
+ What a wonderful way to spend a moment or two
+ To be lying awake and be here talking to you
+ I got something to say I know what I gotta do
+ To be making a change now the moment of truth
+ Why am I feeling so nervous when
+ Things are going so perfect ten?
+ But I know that it's worth it
+ To spend forever with you
+ And so I count to three and get on one knee
+ And I ask you "Darling honestly
+ I've waited all this time just to make it right
+ So I'll ask you (Tonight) will you marry me?
+ Just say 'yes'
+ One word one love one life"
+ A gentle touch of the hand
+ Fingers running through hair
+ Lips pressed to her lips oh I was caught unaware
+ Arms holding me tight tears in both of our eyes
+ What a beautiful way to spend the rest of our lives
+ The sun will reappear burning auburn and red
+ My chest was the pillow green grass knoll was the bed
+ Last night was the night
+ One last moment of truth
+ And what a wonderful way of falling deeper in you
+ Why was I feeling nervous when
+ Things were going so perfect ten?
+ And now I know that it's worth it
+ To spend forever with you
+ And so I count to three and get on one knee
+ And I ask you "Darling honestly
+ I've waited all this time just to make it right
+ So I'll ask you (Tonight) will you marry me?
+ Just say 'yes'
+ One word one love one life"
+ (Your hand in mine) Some things were just meant to be
+ (Hearts intertwined) Some things were just meant to be
+ (In perfect time) Some things were just meant to be
+ (Oh you and I) Some things were just meant to be
+ (Your hand in mine) Some things were just meant to be
+ (Hearts intertwined) Some things were just meant to be
+ (In perfect time) Some things were just meant to be
+ (Oh you and I) Some things were just meant to be</t>
+  </si>
+  <si>
+    <t>I will remember you
+ In the way you'd want me to
+ But it's hard to come to terms right now
+ Sunset looked today
+ As if it knew you'd gone away
+ Now it's night I hear the rain crash down
+ Oh I'd cry but this is more than just my pain
+ Oh I could be a shoulder not a burden
+ And it's time for me to call your son again
+ And say
+ She was the starlight in darkness
+ She was the first bloom in spring
+ An angel with a smile like electric light
+ All the time hit her wings
+ She was the birdsong in morning
+ But now everything here has changed
+ All the world's less beautiful
+ Since you've been away
+ I will remember you
+ With white wine by the barbecue
+ On New York at the birthday doo downtown
+ All that comes to mind
+ When I think about the time
+ Is a memory of laughing out loud
+ Oh I wish that I could take the pain away
+ And just talk to him in person
+ But it's time for me to call your son again
+ And say
+ She was the starlight in darkness
+ She was the first bloom in spring
+ An angel with a smile like electric light
+ All the time hit her wings
+ She was the birdsong in morning
+ But now everything here has changed
+ All the world's less beautiful
+ Since you've been away
+ This doesn't make sense
+ I wish I could change it but
+ I can't do anything
+ My heart is racing
+ And my soul is aching lover
+ She was the starlight in darkness
+ She was the first bloom in spring
+ An angel with a smile like electric light
+ All the time hit her wings
+ She was the birdsong in morning
+ But now everything here has changed
+ All the world's less beautiful
+ Since you've been away
+ The world's less beautiful
+ Since you've been away</t>
+  </si>
+  <si>
+    <t>Welcome to the world
+ I heard your heart beat and lost every word
+ Just stood there quietly taking in the sound
+ Of our love
+ This is gonna hurt
+ But I stand beside you for better or for worse
+ And I will find you whenever you're lost
+ I'll be right here
+ And ooh I know that everything's changing
+ Ooh and I don't wanna miss a thing
+ Ooh I know that life won't ever be the same
+ And this love won't ever go away
+ Welcome to the world
+ Through all the pain you're a diamond in the dirt
+ Don't let them change you words are only words
+ Just like I loved you
+ And yes you were the first
+ Brought a new beginning bright and unreserved
+ A beautiful red flower in the earth
+ Will grow and I know
+ Ooh I know that everything's changing
+ Ooh and I don't wanna miss a thing
+ Ooh I know that life won't ever be the same
+ And this love won't ever go away
+ Welcome to the world
+ Welcome to the world
+ Oh welcome to the world (Welcome to the world)
+ Welcome to the world (Welcome to the world)
+ Ooh I know that everything's changing
+ Ooh and I don't wanna miss a thing
+ Ooh I know that life won't ever be the same
+ And this love won't ever go away
+ You got the kick? (It's just kicks)
+ Is it actually? (Yeah)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peru para
+ Peru para
+ Peru para
+ Peru para
+ Peru para
+ Peru para
+ Peru para
+ Omoge no be so
+ Girl you wan capture my soul
+ Omoge no be so
+ Make we wan wombolobo
+ Peru para
+ Peru peru para
+ I'm loo'
+ Even Peru don dey para
+ Tonight in Jozi (Jozi)
+ I'm in Jozi
+ Mo'n k'orin fun won wan jo si (jo si)
+ I'm not playin' with you I'm not jokin' (jokin')
+ My third album is loadin'
+ Mi okin fa'gbo but I'm on molly
+ I'm on duty but I'm on lowkey
+ They wan do me they wan do mi
+ They wan do me gan they wan do mi
+ Won ni won wa mi
+ Won ni won wa mi
+ I'm in San Francisco jamming
+ Won ni won wa mi
+ Won ni won wa mi
+ I just flew in from Miami
+ Peru (peru) para (para)
+ Peru peru para
+ I'm loo'
+ Even Peru don dey para
+ Pour out the bottle I wanna level up (level up)
+ When I'm with you I nevеr get enough (get еnough)
+ Slow whine I'm not in a rush
+ I can hear music when you're here
+ Tonight we're rolling party 'til closing
+ Since I put the ring on her finger it's still frozen
+ Love in slow motion
+ I wanna feel you over me yeah
+ Somethin' magic in your eyes yeah
+ Girl I love the way you ride it
+ And it happens every time you arrive that's right
+ Girl I want you in my life (yeah)
+ If there's a heaven then it's right here
+ I will never leave your side stay tonight tonight
+ When you wan' see me when you wan' see me
+ I'm in West London this evening
+ Givin' me the feelings no I'm not leavin'
+ Until I fly LA next weekend (next weekend)
+ Peru nah girl I'd rather go find somewhere quiet
+ You'll glow and I'll get lost here in your eyes
+ Omoge no be so
+ Girl you just capture my soul
+ Omoge no be so
+ Make me wanna just take you home
+ Peru para
+ Peru Peru para (woo)
+ I'm loo (loo)
+ Even Peru don dey para
+ Peru para
+ Peru Peru para
+ I'm loo
+ Even Peru don dey para
+ Peru para
+ Peru Peru para
+ I'm loo
+ Even Peru don dey para
+</t>
+  </si>
+  <si>
+    <t>I'm at a party I don't wanna be at
+ And I don't ever wear a suit and tie yeah
+ Wondering if I could sneak out the back
+ Nobody's even looking me in my eyes
+ Then you take my hand
+ Finish my drink say "Shall we dance?" (hell yeah)
+ You know I love you did I ever tell you?
+ You make it better like that
+ Don't think I fit in at this party
+ Everyone's got so much to say (yeah)
+ I always feel like I'm nobody mm
+ Who wants to fit in anyway?
+ 'Cause I don't care when I'm with my baby yeah
+ All the bad things disappear
+ And you're making me feel like maybe I am somebody
+ I can deal with the bad nights
+ When I'm with my baby yeah
+ Ooh ooh ooh ooh ooh ooh
+ 'Cause I don't care as long as you just hold me near
+ You can take me anywhere
+ And you're making me feel like I'm loved by somebody
+ I can deal with the bad nights
+ When I'm with my baby yeah
+ Ooh ooh ooh ooh ooh ooh
+ We at a party we don't wanna be at
+ Tryna talk but we can't hear ourselves
+ Read your lips I'd rather kiss 'em right back
+ With all these people all around
+ I'm crippled with anxiety
+ But I'm told it's where I'm supposed to be
+ You know what? It's kinda crazy 'cause I really don't mind
+ When you make it better like that
+ Don't think we fit in at this party
+ Everyone's got so much to say oh yeah yeah
+ When we walked in I said I'm sorry mm
+ But now I think that we should stay
+ 'Cause I don't care when I'm with my baby yeah
+ All the bad things disappear
+ Yeah you're making me feel like maybe I am somebody
+ I can deal with the bad nights
+ When I'm with my baby yeah
+ Ooh ooh ooh ooh ooh ooh
+ (Oh yeah yeah yeah)
+ 'Cause I don't care as long as you just hold me near
+ You can take me anywhere
+ Yeah you're making me feel like I'm loved by somebody
+ I can deal with the bad nights
+ When I'm with my baby yeah
+ Ooh ooh ooh ooh ooh ooh (no)
+ I don't like nobody but you it's like you're the only one here
+ I don't like nobody but you baby I don't care
+ I don't like nobody but you I hate everyone here
+ I don't like nobody but you baby yeah
+ 'Cause I don't care (don't care)
+ When I'm with my baby yeah (oh yeah)
+ All the bad things disappear (disappear)
+ And you're making me feel like maybe I am somebody (maybe I'm somebody)
+ I can deal with the bad nights (with the bad nights)
+ When I'm with my baby yeah
+ Ooh ooh ooh ooh ooh ooh (ooh yeah yeah)
+ 'Cause I don't care as long as you just hold me near (me near)
+ You can take me anywhere (anywhere anywhere)
+ And you're making me feel like I'm loved by somebody (I'm loved by somebody)
+ I can deal with the bad nights (yeah yeah yeah)
+ When I'm with my baby yeah (oh)
+ Ooh ooh ooh ooh ooh ooh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All you cool people you better leave now
+ 'Cause it's about to happen
+ Friday night and I'm ridin' solo (yeah)
+ When I touch down keep it on the low-low (it's lit)
+ I don't mess with your energy (no)
+ No photos (yeah)
+ So antisocial but I don't care (yeah)
+ Don't give a damn I'm gonna smoke here (yeah pop it)
+ Got a bottle in my hand bring more though (yeah pop it pop it)
+ Got my hat low don't talk to me (straight up)
+ I've been down give me some space
+ You don't know what's in my brain
+ Music loud easin' my pain
+ Yeah yeah yeah yeah
+ Don't touch me don't touch me don't touch me
+ I came to vibe yeah
+ On something on something on something
+ I wanna riot
+ Don't touch me don't touch me don't touch me
+ I came to vibe yeah
+ Won't let nothing come in between me and the night (straight up)
+ Don't touch me don't touch me don't touch me
+ I came to vibe yeah
+ On something on something on something
+ I wanna riot
+ Don't touch me don't touch me don't touch me
+ I came to vibe yeah
+ Won't let nothing come in between me and the night
+ I need room I need room
+ Where you standin' way too close
+ You might catch fumes might catch fumes
+ When I zoom when I zoom
+ Pass out wake up by myself at right past noon right past noon
+ Then I'm doomed
+ (Occupied and moving dolo)
+ (Yeah)
+ Hennessy's drownin' all of my issues (drown)
+ Right before I leave she give me more than just a "Miss you" (yeah)
+ That thing got more back just like my engine I can hit it (in the back)
+ Seen a vision in the boy then we committed
+ I've (it's lit) been lost out inner space
+ You left me right in my place
+ I put you down on my name
+ Yeah yeah yeah yeah
+ Don't touch me don't touch me don't touch me
+ I came to vibe yeah
+ On something on something on something
+ I wanna riot
+ Don't touch me don't touch me don't touch me
+ I came to vibe yeah
+ Won't let nothing come in between me and the night (straight up)
+ Don't touch me don't touch me don't touch me
+ I came to vibe yeah
+ On something on something on something
+ I wanna riot
+ Don't touch me don't touch me don't touch me
+ I came to vibe yeah
+ Won't let nothing come in between me and the night
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I'm feelin' like a bullet jumpin' out a gun
+ I'm feelin' like a winner I feel like the one
+ You're doing somethin' to me
+ You're doing somethin' strange
+ Well jump back talk to me woman
+ You make me wanna make a baby baby uh
+ Supernatural woman supernatural freak
+ Don't know what you're doin' got me feelin' weak
+ Oh I wanna call you fever baby
+ You can set a fire on me
+ Hot damn pop it like a pistol mama
+ You got me down on my knees begging please
+ I'm comin' baby
+ I'm gunnin' for you yeah
+ Locked loaded shoot my shot tonight
+ I'm comin' baby
+ I'm gunnin' for you
+ Pull my trigger let me blow your mind
+ You red leather rocket you little foxy queen
+ Everybody's watching pretty little thing
+ Baby tell me what's your fantasy?
+ Come closer let's talk about it
+ You want white lines in a limousine
+ Whipped cream and everything in between yeah
+ I'm comin' baby
+ I'm gunnin' for you yeah
+ Locked loaded shoot my shot tonight
+ I'm comin' baby
+ I'm gunnin' for you
+ Pull my trigger let me blow your mind
+ I'm comin' baby
+ I'm comin' baby
+ I'm gunnin' for you yeah
+ Locked loaded shoot my shot tonight
+ I'm comin' baby
+ I'm gunnin' for you
+ Pull my trigger let me blow your mind
+</t>
   </si>
 </sst>
 </file>
@@ -1536,10 +1818,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1779,10 +2059,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F139"/>
+  <dimension ref="A1:F138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="F127" sqref="F127"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="H137" sqref="H137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2018,7 +2298,7 @@
         <v>28</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E12" s="2">
         <v>0.17916666666666667</v>
@@ -2044,7 +2324,7 @@
         <v>0.14166666666666666</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -2084,7 +2364,7 @@
         <v>0.13680555555555554</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -2124,7 +2404,7 @@
         <v>0.14305555555555557</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -2178,7 +2458,7 @@
         <v>42</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E20" s="2">
         <v>0.12847222222222224</v>
@@ -2238,7 +2518,7 @@
         <v>48</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E23" s="2">
         <v>0.36527777777777781</v>
@@ -2258,7 +2538,7 @@
         <v>50</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E24" s="2">
         <v>0.19444444444444445</v>
@@ -2338,7 +2618,7 @@
         <v>58</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E28" s="2">
         <v>0.12847222222222224</v>
@@ -2438,7 +2718,7 @@
         <v>68</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E33" s="2">
         <v>0.15277777777777776</v>
@@ -2484,7 +2764,7 @@
         <v>0.13125000000000001</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -2578,7 +2858,7 @@
         <v>81</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E40" s="2">
         <v>0.15833333333333333</v>
@@ -2604,7 +2884,7 @@
         <v>0.16874999999999998</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -2638,7 +2918,7 @@
         <v>86</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E43" s="2">
         <v>0.17986111111111111</v>
@@ -2658,7 +2938,7 @@
         <v>88</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E44" s="2">
         <v>0.15902777777777777</v>
@@ -2678,10 +2958,10 @@
         <v>90</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>248</v>
+        <v>18</v>
       </c>
       <c r="E45" s="2">
-        <v>0.16250000000000001</v>
+        <v>0.17361111111111113</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>91</v>
@@ -2698,10 +2978,10 @@
         <v>92</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>18</v>
+        <v>228</v>
       </c>
       <c r="E46" s="2">
-        <v>0.17361111111111113</v>
+        <v>0.1388888888888889</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>93</v>
@@ -2718,10 +2998,10 @@
         <v>94</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>230</v>
+        <v>18</v>
       </c>
       <c r="E47" s="2">
-        <v>0.1388888888888889</v>
+        <v>0.1423611111111111</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>95</v>
@@ -2738,13 +3018,13 @@
         <v>96</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="E48" s="2">
-        <v>0.1423611111111111</v>
+        <v>0.1388888888888889</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>97</v>
+        <v>254</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -2755,16 +3035,16 @@
         <v>5</v>
       </c>
       <c r="C49" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E49" s="2">
+        <v>0.15833333333333333</v>
+      </c>
+      <c r="F49" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E49" s="2">
-        <v>0.1388888888888889</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -2778,13 +3058,13 @@
         <v>99</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>18</v>
+        <v>100</v>
       </c>
       <c r="E50" s="2">
-        <v>0.15833333333333333</v>
+        <v>0.22777777777777777</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -2795,16 +3075,16 @@
         <v>5</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>102</v>
+        <v>31</v>
       </c>
       <c r="E51" s="2">
-        <v>0.22777777777777777</v>
+        <v>0.13680555555555554</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>103</v>
+        <v>255</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -2815,16 +3095,16 @@
         <v>5</v>
       </c>
       <c r="C52" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E52" s="2">
+        <v>0.28055555555555556</v>
+      </c>
+      <c r="F52" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E52" s="2">
-        <v>0.13680555555555554</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -2838,10 +3118,10 @@
         <v>105</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>18</v>
+        <v>228</v>
       </c>
       <c r="E53" s="2">
-        <v>0.28055555555555556</v>
+        <v>0.1388888888888889</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>106</v>
@@ -2855,16 +3135,16 @@
         <v>5</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>230</v>
+        <v>31</v>
       </c>
       <c r="E54" s="2">
-        <v>0.1388888888888889</v>
+        <v>0.14722222222222223</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>108</v>
+        <v>256</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -2875,16 +3155,16 @@
         <v>5</v>
       </c>
       <c r="C55" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D55" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E55" s="2">
-        <v>0.14722222222222223</v>
+        <v>0.13194444444444445</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>259</v>
+        <v>111</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -2895,10 +3175,10 @@
         <v>5</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>112</v>
+        <v>31</v>
       </c>
       <c r="E56" s="2">
         <v>0.13194444444444445</v>
@@ -2921,7 +3201,7 @@
         <v>31</v>
       </c>
       <c r="E57" s="2">
-        <v>0.13194444444444445</v>
+        <v>0.10416666666666667</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>115</v>
@@ -2938,10 +3218,10 @@
         <v>116</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>31</v>
+        <v>228</v>
       </c>
       <c r="E58" s="2">
-        <v>0.10416666666666667</v>
+        <v>0.12430555555555556</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>117</v>
@@ -2958,10 +3238,10 @@
         <v>118</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>230</v>
+        <v>18</v>
       </c>
       <c r="E59" s="2">
-        <v>0.12430555555555556</v>
+        <v>0.13194444444444445</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>119</v>
@@ -2978,10 +3258,10 @@
         <v>120</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>18</v>
+        <v>228</v>
       </c>
       <c r="E60" s="2">
-        <v>0.13194444444444445</v>
+        <v>0.19097222222222221</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>121</v>
@@ -2998,10 +3278,10 @@
         <v>122</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>230</v>
+        <v>31</v>
       </c>
       <c r="E61" s="2">
-        <v>0.19097222222222221</v>
+        <v>0.14166666666666666</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>123</v>
@@ -3015,16 +3295,16 @@
         <v>5</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>31</v>
+        <v>228</v>
       </c>
       <c r="E62" s="2">
-        <v>0.14166666666666666</v>
+        <v>0.13541666666666666</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -3038,13 +3318,13 @@
         <v>129</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>230</v>
+        <v>130</v>
       </c>
       <c r="E63" s="2">
-        <v>0.13541666666666666</v>
+        <v>0.1763888888888889</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -3055,13 +3335,13 @@
         <v>5</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>132</v>
+        <v>228</v>
       </c>
       <c r="E64" s="2">
-        <v>0.1763888888888889</v>
+        <v>0.16250000000000001</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>133</v>
@@ -3078,10 +3358,10 @@
         <v>134</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>230</v>
+        <v>18</v>
       </c>
       <c r="E65" s="2">
-        <v>0.16250000000000001</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>135</v>
@@ -3101,7 +3381,7 @@
         <v>18</v>
       </c>
       <c r="E66" s="2">
-        <v>0.16666666666666666</v>
+        <v>0.16319444444444445</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>137</v>
@@ -3118,10 +3398,10 @@
         <v>138</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>18</v>
+        <v>130</v>
       </c>
       <c r="E67" s="2">
-        <v>0.16319444444444445</v>
+        <v>0.16944444444444443</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>139</v>
@@ -3138,10 +3418,10 @@
         <v>140</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E68" s="2">
-        <v>0.16944444444444443</v>
+        <v>0.14583333333333334</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>141</v>
@@ -3157,11 +3437,11 @@
       <c r="C69" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D69" s="1" t="s">
-        <v>127</v>
+      <c r="D69" t="s">
+        <v>227</v>
       </c>
       <c r="E69" s="2">
-        <v>0.14583333333333334</v>
+        <v>0.17222222222222225</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>143</v>
@@ -3177,11 +3457,11 @@
       <c r="C70" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D70" t="s">
-        <v>229</v>
+      <c r="D70" s="1" t="s">
+        <v>228</v>
       </c>
       <c r="E70" s="2">
-        <v>0.17222222222222225</v>
+        <v>0.16874999999999998</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>145</v>
@@ -3198,10 +3478,10 @@
         <v>146</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="E71" s="2">
-        <v>0.16874999999999998</v>
+        <v>125</v>
+      </c>
+      <c r="E71" s="3">
+        <v>0.14305555555555557</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>147</v>
@@ -3218,10 +3498,10 @@
         <v>148</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E72" s="3">
-        <v>0.14305555555555557</v>
+        <v>18</v>
+      </c>
+      <c r="E72" s="2">
+        <v>0.1277777777777778</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>149</v>
@@ -3238,13 +3518,13 @@
         <v>150</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>18</v>
+        <v>151</v>
       </c>
       <c r="E73" s="2">
-        <v>0.1277777777777778</v>
+        <v>0.15138888888888888</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -3255,13 +3535,13 @@
         <v>5</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>153</v>
+        <v>125</v>
       </c>
       <c r="E74" s="2">
-        <v>0.15138888888888888</v>
+        <v>0.1763888888888889</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>154</v>
@@ -3278,10 +3558,10 @@
         <v>155</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="E75" s="2">
-        <v>0.1763888888888889</v>
+        <v>0.16527777777777777</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>156</v>
@@ -3298,10 +3578,10 @@
         <v>157</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="E76" s="2">
-        <v>0.16527777777777777</v>
+        <v>0.16041666666666668</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>158</v>
@@ -3318,10 +3598,10 @@
         <v>159</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>127</v>
+        <v>151</v>
       </c>
       <c r="E77" s="2">
-        <v>0.16041666666666668</v>
+        <v>0.18611111111111112</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>160</v>
@@ -3338,10 +3618,10 @@
         <v>161</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>153</v>
+        <v>125</v>
       </c>
       <c r="E78" s="2">
-        <v>0.18611111111111112</v>
+        <v>0.13819444444444443</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>162</v>
@@ -3358,10 +3638,10 @@
         <v>163</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="E79" s="2">
-        <v>0.13819444444444443</v>
+        <v>0.11319444444444444</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>164</v>
@@ -3378,13 +3658,13 @@
         <v>165</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>132</v>
+        <v>100</v>
       </c>
       <c r="E80" s="2">
-        <v>0.11319444444444444</v>
+        <v>0.18819444444444444</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>166</v>
+        <v>257</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -3395,16 +3675,16 @@
         <v>5</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E81" s="2">
-        <v>0.18819444444444444</v>
+        <v>0.1763888888888889</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -3415,16 +3695,16 @@
         <v>5</v>
       </c>
       <c r="C82" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E82" s="2">
+        <v>0.12708333333333333</v>
+      </c>
+      <c r="F82" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E82" s="2">
-        <v>0.1763888888888889</v>
-      </c>
-      <c r="F82" s="1" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -3438,13 +3718,13 @@
         <v>169</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>132</v>
+        <v>100</v>
       </c>
       <c r="E83" s="2">
-        <v>0.12708333333333333</v>
+        <v>0.22916666666666666</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>170</v>
+        <v>259</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -3455,16 +3735,16 @@
         <v>5</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
       <c r="E84" s="2">
-        <v>0.22916666666666666</v>
+        <v>9.9999999999999992E-2</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -3475,16 +3755,16 @@
         <v>5</v>
       </c>
       <c r="C85" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E85" s="2">
+        <v>0.15416666666666667</v>
+      </c>
+      <c r="F85" s="1" t="s">
         <v>172</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E85" s="2">
-        <v>9.9999999999999992E-2</v>
-      </c>
-      <c r="F85" s="1" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -3498,10 +3778,10 @@
         <v>173</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E86" s="2">
-        <v>0.15416666666666667</v>
+        <v>0.13958333333333334</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>174</v>
@@ -3518,10 +3798,10 @@
         <v>175</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E87" s="2">
-        <v>0.13958333333333334</v>
+        <v>0.16874999999999998</v>
       </c>
       <c r="F87" s="1" t="s">
         <v>176</v>
@@ -3538,10 +3818,10 @@
         <v>177</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E88" s="2">
-        <v>0.16874999999999998</v>
+        <v>0.18124999999999999</v>
       </c>
       <c r="F88" s="1" t="s">
         <v>178</v>
@@ -3558,13 +3838,13 @@
         <v>179</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>102</v>
+        <v>180</v>
       </c>
       <c r="E89" s="2">
-        <v>0.18124999999999999</v>
+        <v>0.12569444444444444</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -3575,16 +3855,16 @@
         <v>5</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E90" s="2">
         <v>0.12569444444444444</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -3595,16 +3875,16 @@
         <v>5</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E91" s="2">
-        <v>0.12569444444444444</v>
+        <v>0.16458333333333333</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>186</v>
+        <v>261</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -3615,16 +3895,16 @@
         <v>5</v>
       </c>
       <c r="C92" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E92" s="2">
+        <v>8.8888888888888892E-2</v>
+      </c>
+      <c r="F92" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="E92" s="2">
-        <v>0.16458333333333333</v>
-      </c>
-      <c r="F92" s="1" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -3638,10 +3918,10 @@
         <v>188</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E93" s="2">
-        <v>8.8888888888888892E-2</v>
+        <v>0.17916666666666667</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>189</v>
@@ -3658,10 +3938,10 @@
         <v>190</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E94" s="2">
-        <v>0.17916666666666667</v>
+        <v>0.15972222222222224</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>191</v>
@@ -3678,10 +3958,10 @@
         <v>192</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E95" s="2">
-        <v>0.15972222222222224</v>
+        <v>0.12569444444444444</v>
       </c>
       <c r="F95" s="1" t="s">
         <v>193</v>
@@ -3698,10 +3978,10 @@
         <v>194</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E96" s="2">
-        <v>0.12569444444444444</v>
+        <v>0.13125000000000001</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>195</v>
@@ -3718,10 +3998,10 @@
         <v>196</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E97" s="2">
-        <v>0.13125000000000001</v>
+        <v>0.11597222222222221</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>197</v>
@@ -3738,10 +4018,10 @@
         <v>198</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E98" s="2">
-        <v>0.11597222222222221</v>
+        <v>8.819444444444445E-2</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>199</v>
@@ -3758,10 +4038,10 @@
         <v>200</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E99" s="2">
-        <v>8.819444444444445E-2</v>
+        <v>0.12083333333333333</v>
       </c>
       <c r="F99" s="1" t="s">
         <v>201</v>
@@ -3778,10 +4058,10 @@
         <v>202</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E100" s="2">
-        <v>0.12083333333333333</v>
+        <v>0.18124999999999999</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>203</v>
@@ -3798,10 +4078,10 @@
         <v>204</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E101" s="2">
-        <v>0.18124999999999999</v>
+        <v>0.21805555555555556</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>205</v>
@@ -3818,10 +4098,10 @@
         <v>206</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E102" s="2">
-        <v>0.21805555555555556</v>
+        <v>0.14583333333333334</v>
       </c>
       <c r="F102" s="1" t="s">
         <v>207</v>
@@ -3838,10 +4118,10 @@
         <v>208</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E103" s="2">
-        <v>0.14583333333333334</v>
+        <v>0.12083333333333333</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>209</v>
@@ -3858,10 +4138,10 @@
         <v>210</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E104" s="2">
-        <v>0.12083333333333333</v>
+        <v>0.16180555555555556</v>
       </c>
       <c r="F104" s="1" t="s">
         <v>211</v>
@@ -3878,13 +4158,13 @@
         <v>212</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E105" s="2">
-        <v>0.16180555555555556</v>
+        <v>0.13333333333333333</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>213</v>
+        <v>262</v>
       </c>
     </row>
     <row r="106" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -3895,16 +4175,16 @@
         <v>5</v>
       </c>
       <c r="C106" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E106" s="2">
+        <v>9.0972222222222218E-2</v>
+      </c>
+      <c r="F106" s="1" t="s">
         <v>214</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="E106" s="2">
-        <v>0.13333333333333333</v>
-      </c>
-      <c r="F106" s="1" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="107" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -3918,10 +4198,10 @@
         <v>215</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E107" s="2">
-        <v>9.0972222222222218E-2</v>
+        <v>8.1944444444444445E-2</v>
       </c>
       <c r="F107" s="1" t="s">
         <v>216</v>
@@ -3938,10 +4218,10 @@
         <v>217</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E108" s="2">
-        <v>8.1944444444444445E-2</v>
+        <v>0.21875</v>
       </c>
       <c r="F108" s="1" t="s">
         <v>218</v>
@@ -3958,10 +4238,10 @@
         <v>219</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E109" s="2">
-        <v>0.21875</v>
+        <v>0.11944444444444445</v>
       </c>
       <c r="F109" s="1" t="s">
         <v>220</v>
@@ -3978,10 +4258,10 @@
         <v>221</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E110" s="2">
-        <v>0.11944444444444445</v>
+        <v>0.14444444444444446</v>
       </c>
       <c r="F110" s="1" t="s">
         <v>222</v>
@@ -3998,10 +4278,10 @@
         <v>223</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E111" s="2">
-        <v>0.14444444444444446</v>
+        <v>6.7361111111111108E-2</v>
       </c>
       <c r="F111" s="1" t="s">
         <v>224</v>
@@ -4018,16 +4298,16 @@
         <v>225</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E112" s="2">
-        <v>6.7361111111111108E-2</v>
-      </c>
-      <c r="F112" s="1" t="s">
+        <v>5.6944444444444443E-2</v>
+      </c>
+      <c r="F112" s="4" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -4035,16 +4315,16 @@
         <v>5</v>
       </c>
       <c r="C113" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="D113" t="s">
         <v>227</v>
       </c>
-      <c r="D113" s="1" t="s">
-        <v>185</v>
-      </c>
       <c r="E113" s="2">
-        <v>5.6944444444444443E-2</v>
+        <v>0.13541666666666666</v>
       </c>
       <c r="F113" s="5" t="s">
-        <v>228</v>
+        <v>263</v>
       </c>
     </row>
     <row r="114" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4055,16 +4335,16 @@
         <v>5</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D114" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E114" s="2">
-        <v>0.13541666666666666</v>
-      </c>
-      <c r="F114" s="4" t="s">
-        <v>266</v>
+        <v>0.14375000000000002</v>
+      </c>
+      <c r="F114" s="5" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="115" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4075,16 +4355,16 @@
         <v>5</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D115" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E115" s="2">
-        <v>0.14375000000000002</v>
-      </c>
-      <c r="F115" s="4" t="s">
-        <v>267</v>
+        <v>0.12847222222222224</v>
+      </c>
+      <c r="F115" s="5" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="116" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4095,16 +4375,16 @@
         <v>5</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D116" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E116" s="2">
-        <v>0.12847222222222224</v>
-      </c>
-      <c r="F116" s="4" t="s">
-        <v>268</v>
+        <v>0.15972222222222224</v>
+      </c>
+      <c r="F116" s="5" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="117" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4114,17 +4394,17 @@
       <c r="B117" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C117" s="1" t="s">
-        <v>234</v>
+      <c r="C117" s="4" t="s">
+        <v>233</v>
       </c>
       <c r="D117" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E117" s="2">
-        <v>0.15972222222222224</v>
-      </c>
-      <c r="F117" s="4" t="s">
-        <v>269</v>
+        <v>0.16388888888888889</v>
+      </c>
+      <c r="F117" s="5" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="118" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4134,17 +4414,17 @@
       <c r="B118" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C118" s="5" t="s">
-        <v>235</v>
+      <c r="C118" s="1" t="s">
+        <v>234</v>
       </c>
       <c r="D118" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E118" s="2">
-        <v>0.16388888888888889</v>
-      </c>
-      <c r="F118" s="4" t="s">
-        <v>270</v>
+        <v>0.12847222222222224</v>
+      </c>
+      <c r="F118" s="5" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="119" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4155,16 +4435,16 @@
         <v>5</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D119" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E119" s="2">
-        <v>0.12847222222222224</v>
-      </c>
-      <c r="F119" s="4" t="s">
-        <v>271</v>
+        <v>0.15486111111111112</v>
+      </c>
+      <c r="F119" s="5" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="120" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4175,16 +4455,16 @@
         <v>5</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D120" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E120" s="2">
-        <v>0.15486111111111112</v>
-      </c>
-      <c r="F120" s="4" t="s">
-        <v>272</v>
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="F120" s="5" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="121" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4195,16 +4475,16 @@
         <v>5</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D121" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E121" s="2">
-        <v>0.14583333333333334</v>
-      </c>
-      <c r="F121" s="4" t="s">
-        <v>273</v>
+        <v>0.10625</v>
+      </c>
+      <c r="F121" s="5" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="122" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4215,16 +4495,16 @@
         <v>5</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D122" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E122" s="2">
-        <v>0.10625</v>
-      </c>
-      <c r="F122" s="4" t="s">
-        <v>274</v>
+        <v>0.14097222222222222</v>
+      </c>
+      <c r="F122" s="5" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="123" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4235,16 +4515,16 @@
         <v>5</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D123" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E123" s="2">
-        <v>0.14097222222222222</v>
-      </c>
-      <c r="F123" s="4" t="s">
-        <v>275</v>
+        <v>0.13194444444444445</v>
+      </c>
+      <c r="F123" s="5" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="124" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4255,16 +4535,16 @@
         <v>5</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D124" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E124" s="2">
-        <v>0.13194444444444445</v>
-      </c>
-      <c r="F124" s="4" t="s">
-        <v>276</v>
+        <v>0.14930555555555555</v>
+      </c>
+      <c r="F124" s="5" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="125" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4275,16 +4555,16 @@
         <v>5</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D125" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E125" s="2">
-        <v>0.14930555555555555</v>
-      </c>
-      <c r="F125" s="4" t="s">
-        <v>277</v>
+        <v>0.17986111111111111</v>
+      </c>
+      <c r="F125" s="5" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="126" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4295,16 +4575,16 @@
         <v>5</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D126" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E126" s="2">
-        <v>0.17986111111111111</v>
-      </c>
-      <c r="F126" s="4" t="s">
-        <v>278</v>
+        <v>0.14652777777777778</v>
+      </c>
+      <c r="F126" s="5" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="127" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4315,16 +4595,16 @@
         <v>5</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>244</v>
+        <v>107</v>
       </c>
       <c r="D127" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E127" s="2">
-        <v>0.14652777777777778</v>
-      </c>
-      <c r="F127" s="4" t="s">
-        <v>279</v>
+        <v>0.16041666666666668</v>
+      </c>
+      <c r="F127" s="5" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="128" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4335,13 +4615,16 @@
         <v>5</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>109</v>
+        <v>243</v>
       </c>
       <c r="D128" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E128" s="2">
-        <v>0.16041666666666668</v>
+        <v>0.14861111111111111</v>
+      </c>
+      <c r="F128" s="5" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="129" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4352,13 +4635,16 @@
         <v>5</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D129" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E129" s="2">
-        <v>0.14861111111111111</v>
+        <v>0.12222222222222223</v>
+      </c>
+      <c r="F129" s="5" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="130" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4369,16 +4655,19 @@
         <v>5</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D130" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E130" s="2">
-        <v>0.12222222222222223</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.12986111111111112</v>
+      </c>
+      <c r="F130" s="5" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -4386,16 +4675,19 @@
         <v>5</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="D131" t="s">
-        <v>229</v>
+        <v>124</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>228</v>
       </c>
       <c r="E131" s="2">
-        <v>0.12986111111111112</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+        <v>0.15555555555555556</v>
+      </c>
+      <c r="F131" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -4403,16 +4695,16 @@
         <v>5</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>126</v>
+        <v>246</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>230</v>
+        <v>31</v>
       </c>
       <c r="E132" s="2">
-        <v>0.15555555555555556</v>
-      </c>
-      <c r="F132" s="1" t="s">
-        <v>128</v>
+        <v>0.15208333333333332</v>
+      </c>
+      <c r="F132" s="5" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="133" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4423,13 +4715,16 @@
         <v>5</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E133" s="2">
-        <v>0.15208333333333332</v>
+        <v>0.11180555555555556</v>
+      </c>
+      <c r="F133" s="5" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="134" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4440,31 +4735,23 @@
         <v>5</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D134" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E134" s="2">
-        <v>0.11180555555555556</v>
+        <v>0.1451388888888889</v>
+      </c>
+      <c r="F134" s="5" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="135" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A135" s="1">
-        <v>133</v>
-      </c>
-      <c r="B135" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C135" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="D135" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E135" s="2">
-        <v>0.1451388888888889</v>
-      </c>
+      <c r="B135" s="1"/>
+      <c r="C135" s="1"/>
+      <c r="D135" s="1"/>
+      <c r="E135" s="2"/>
     </row>
     <row r="136" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B136" s="1"/>
@@ -4473,21 +4760,15 @@
       <c r="E136" s="2"/>
     </row>
     <row r="137" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B137" s="1"/>
       <c r="C137" s="1"/>
       <c r="D137" s="1"/>
-      <c r="E137" s="2"/>
     </row>
     <row r="138" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C138" s="1"/>
       <c r="D138" s="1"/>
     </row>
-    <row r="139" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C139" s="1"/>
-      <c r="D139" s="1"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:F135"/>
+  <autoFilter ref="A1:F134"/>
   <conditionalFormatting sqref="C1:C1048576">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>

</xml_diff>